<commit_message>
Switch back to 7% discount rate, adapt tax credits to reflect different discount rates for different technologies
</commit_message>
<xml_diff>
--- a/data/tax_credits/tax_credits_calculations.xlsx
+++ b/data/tax_credits/tax_credits_calculations.xlsx
@@ -321,7 +321,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -380,22 +380,22 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>0.08</v>
+        <v>0.07</v>
       </c>
       <c r="F2" s="2" t="n">
-        <f aca="false">$E$2/(1-(1/(1+$E$2)^C2))</f>
-        <v>0.0807979487636457</v>
+        <f aca="false">E2/(1-(1/(1+E2)^C2))</f>
+        <v>0.0712292255000195</v>
       </c>
       <c r="G2" s="2" t="n">
         <f aca="false">F2/(1-(1/(1+F2)^D2))</f>
-        <v>0.160611279854251</v>
+        <v>0.154290036689704</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>0.2574</v>
       </c>
       <c r="I2" s="3" t="n">
         <f aca="false">B2/(1-$H$2)*F2/G2</f>
-        <v>-10.1615651675138</v>
+        <v>-9.32516777004039</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -411,17 +411,20 @@
       <c r="D3" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="E3" s="1" t="n">
+        <v>0.07</v>
+      </c>
       <c r="F3" s="2" t="n">
-        <f aca="false">$E$2/(1-(1/(1+$E$2)^C3))</f>
-        <v>0.0807979487636457</v>
+        <f aca="false">E3/(1-(1/(1+E3)^C3))</f>
+        <v>0.0712292255000195</v>
       </c>
       <c r="G3" s="2" t="n">
         <f aca="false">F3/(1-(1/(1+F3)^D3))</f>
-        <v>0.149566305987116</v>
+        <v>0.143187579596091</v>
       </c>
       <c r="I3" s="3" t="n">
         <f aca="false">B3/(1-$H$2)*F3/G3</f>
-        <v>-20.0052653761814</v>
+        <v>-18.4217389243225</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -437,17 +440,20 @@
       <c r="D4" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="E4" s="1" t="n">
+        <v>0.07</v>
+      </c>
       <c r="F4" s="2" t="n">
-        <f aca="false">$E$2/(1-(1/(1+$E$2)^C4))</f>
-        <v>0.0888274333872723</v>
+        <f aca="false">E4/(1-(1/(1+E4)^C4))</f>
+        <v>0.0805864035111112</v>
       </c>
       <c r="G4" s="2" t="n">
         <f aca="false">F4/(1-(1/(1+F4)^D4))</f>
-        <v>0.155016799199575</v>
+        <v>0.149423903774895</v>
       </c>
       <c r="I4" s="3" t="n">
         <f aca="false">B4/(1-$H$2)*F4/G4</f>
-        <v>-21.2200350676872</v>
+        <v>-19.9719028411147</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -463,17 +469,20 @@
       <c r="D5" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="E5" s="1" t="n">
+        <v>0.07</v>
+      </c>
       <c r="F5" s="2" t="n">
-        <f aca="false">$E$2/(1-(1/(1+$E$2)^C5))</f>
-        <v>0.0888274333872723</v>
+        <f aca="false">E5/(1-(1/(1+E5)^C5))</f>
+        <v>0.0805864035111112</v>
       </c>
       <c r="G5" s="2" t="n">
         <f aca="false">F5/(1-(1/(1+F5)^D5))</f>
-        <v>0.155016799199575</v>
+        <v>0.149423903774895</v>
       </c>
       <c r="I5" s="3" t="n">
         <f aca="false">B5/(1-$H$2)*F5/G5</f>
-        <v>-21.2200350676872</v>
+        <v>-19.9719028411147</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -489,17 +498,20 @@
       <c r="D6" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="E6" s="1" t="n">
+        <v>0.07</v>
+      </c>
       <c r="F6" s="2" t="n">
-        <f aca="false">$E$2/(1-(1/(1+$E$2)^C6))</f>
-        <v>0.0858032645606798</v>
+        <f aca="false">E6/(1-(1/(1+E6)^C6))</f>
+        <v>0.0772339596490032</v>
       </c>
       <c r="G6" s="2" t="n">
         <f aca="false">F6/(1-(1/(1+F6)^D6))</f>
-        <v>0.152953623736828</v>
+        <v>0.147175489847447</v>
       </c>
       <c r="I6" s="3" t="n">
         <f aca="false">B6/(1-$H$2)*F6/G6</f>
-        <v>-20.7740795387224</v>
+        <v>-19.4334792027051</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -515,17 +527,20 @@
       <c r="D7" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="E7" s="1" t="n">
+        <v>0.07</v>
+      </c>
       <c r="F7" s="2" t="n">
-        <f aca="false">$E$2/(1-(1/(1+$E$2)^C7))</f>
-        <v>0.0914480962075644</v>
+        <f aca="false">E7/(1-(1/(1+E7)^C7))</f>
+        <v>0.0834257340177891</v>
       </c>
       <c r="G7" s="2" t="n">
         <f aca="false">F7/(1-(1/(1+F7)^D7))</f>
-        <v>0.156814693193101</v>
+        <v>0.151340354350156</v>
       </c>
       <c r="I7" s="3" t="n">
         <f aca="false">B7/(1-$H$2)*F7/G7</f>
-        <v>-21.5956193999951</v>
+        <v>-20.4137616145153</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -541,17 +556,20 @@
       <c r="D8" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="E8" s="1" t="n">
+        <v>0.07</v>
+      </c>
       <c r="F8" s="2" t="n">
-        <f aca="false">$E$2/(1-(1/(1+$E$2)^C8))</f>
-        <v>0.0914480962075644</v>
+        <f aca="false">E8/(1-(1/(1+E8)^C8))</f>
+        <v>0.0834257340177891</v>
       </c>
       <c r="G8" s="2" t="n">
         <f aca="false">F8/(1-(1/(1+F8)^D8))</f>
-        <v>0.156814693193101</v>
+        <v>0.151340354350156</v>
       </c>
       <c r="I8" s="3" t="n">
         <f aca="false">B8/(1-$H$2)*F8/G8</f>
-        <v>-21.5956193999951</v>
+        <v>-20.4137616145153</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -567,17 +585,20 @@
       <c r="D9" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="E9" s="1" t="n">
+        <v>0.07</v>
+      </c>
       <c r="F9" s="2" t="n">
-        <f aca="false">$E$2/(1-(1/(1+$E$2)^C9))</f>
-        <v>0.0914480962075644</v>
+        <f aca="false">E9/(1-(1/(1+E9)^C9))</f>
+        <v>0.0834257340177891</v>
       </c>
       <c r="G9" s="2" t="n">
         <f aca="false">F9/(1-(1/(1+F9)^D9))</f>
-        <v>0.156814693193101</v>
+        <v>0.151340354350156</v>
       </c>
       <c r="I9" s="3" t="n">
         <f aca="false">B9/(1-$H$2)*F9/G9</f>
-        <v>-21.5956193999951</v>
+        <v>-20.4137616145153</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -593,17 +614,20 @@
       <c r="D10" s="1" t="n">
         <v>12</v>
       </c>
+      <c r="E10" s="1" t="n">
+        <v>0.07</v>
+      </c>
       <c r="F10" s="2" t="n">
-        <f aca="false">$E$2/(1-(1/(1+$E$2)^C10))</f>
-        <v>0.101852208823151</v>
+        <f aca="false">E10/(1-(1/(1+E10)^C10))</f>
+        <v>0.0943929257432557</v>
       </c>
       <c r="G10" s="2" t="n">
         <f aca="false">F10/(1-(1/(1+F10)^D10))</f>
-        <v>0.148097507714605</v>
+        <v>0.142756193054826</v>
       </c>
       <c r="I10" s="3" t="n">
         <f aca="false">B10/(1-$H$2)*F10/G10</f>
-        <v>-78.7202895097239</v>
+        <v>-75.6847656176249</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -619,17 +643,20 @@
       <c r="D11" s="1" t="n">
         <v>12</v>
       </c>
+      <c r="E11" s="1" t="n">
+        <v>0.07</v>
+      </c>
       <c r="F11" s="2" t="n">
-        <f aca="false">$E$2/(1-(1/(1+$E$2)^C11))</f>
-        <v>0.101852208823151</v>
+        <f aca="false">E11/(1-(1/(1+E11)^C11))</f>
+        <v>0.0943929257432557</v>
       </c>
       <c r="G11" s="2" t="n">
         <f aca="false">F11/(1-(1/(1+F11)^D11))</f>
-        <v>0.148097507714605</v>
+        <v>0.142756193054826</v>
       </c>
       <c r="I11" s="3" t="n">
         <f aca="false">B11/(1-$H$2)*F11/G11</f>
-        <v>-78.7202895097239</v>
+        <v>-75.6847656176249</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -645,17 +672,20 @@
       <c r="D12" s="1" t="n">
         <v>12</v>
       </c>
+      <c r="E12" s="1" t="n">
+        <v>0.07</v>
+      </c>
       <c r="F12" s="2" t="n">
-        <f aca="false">$E$2/(1-(1/(1+$E$2)^C12))</f>
-        <v>0.101852208823151</v>
+        <f aca="false">E12/(1-(1/(1+E12)^C12))</f>
+        <v>0.0943929257432557</v>
       </c>
       <c r="G12" s="2" t="n">
         <f aca="false">F12/(1-(1/(1+F12)^D12))</f>
-        <v>0.148097507714605</v>
+        <v>0.142756193054826</v>
       </c>
       <c r="I12" s="3" t="n">
         <f aca="false">B12/(1-$H$2)*F12/G12</f>
-        <v>-78.7202895097239</v>
+        <v>-75.6847656176249</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -671,17 +701,20 @@
       <c r="D13" s="1" t="n">
         <v>12</v>
       </c>
+      <c r="E13" s="1" t="n">
+        <v>0.07</v>
+      </c>
       <c r="F13" s="2" t="n">
-        <f aca="false">$E$2/(1-(1/(1+$E$2)^C13))</f>
-        <v>0.101852208823151</v>
+        <f aca="false">E13/(1-(1/(1+E13)^C13))</f>
+        <v>0.0943929257432557</v>
       </c>
       <c r="G13" s="2" t="n">
         <f aca="false">F13/(1-(1/(1+F13)^D13))</f>
-        <v>0.148097507714605</v>
+        <v>0.142756193054826</v>
       </c>
       <c r="I13" s="3" t="n">
         <f aca="false">B13/(1-$H$2)*F13/G13</f>
-        <v>-78.7202895097239</v>
+        <v>-75.6847656176249</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -697,17 +730,20 @@
       <c r="D14" s="1" t="n">
         <v>12</v>
       </c>
+      <c r="E14" s="1" t="n">
+        <v>0.07</v>
+      </c>
       <c r="F14" s="2" t="n">
-        <f aca="false">$E$2/(1-(1/(1+$E$2)^C14))</f>
-        <v>0.101852208823151</v>
+        <f aca="false">E14/(1-(1/(1+E14)^C14))</f>
+        <v>0.0943929257432557</v>
       </c>
       <c r="G14" s="2" t="n">
         <f aca="false">F14/(1-(1/(1+F14)^D14))</f>
-        <v>0.148097507714605</v>
+        <v>0.142756193054826</v>
       </c>
       <c r="I14" s="3" t="n">
         <f aca="false">B14/(1-$H$2)*F14/G14</f>
-        <v>-78.7202895097239</v>
+        <v>-75.6847656176249</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -723,17 +759,20 @@
       <c r="D15" s="1" t="n">
         <v>12</v>
       </c>
+      <c r="E15" s="1" t="n">
+        <v>0.1</v>
+      </c>
       <c r="F15" s="2" t="n">
-        <f aca="false">$E$2/(1-(1/(1+$E$2)^C15))</f>
-        <v>0.0888274333872723</v>
+        <f aca="false">E15/(1-(1/(1+E15)^C15))</f>
+        <v>0.106079248252634</v>
       </c>
       <c r="G15" s="2" t="n">
         <f aca="false">F15/(1-(1/(1+F15)^D15))</f>
-        <v>0.138826828064813</v>
+        <v>0.151161597709284</v>
       </c>
       <c r="I15" s="3" t="n">
         <f aca="false">B15/(1-$H$2)*F15/G15</f>
-        <v>-155.092670086866</v>
+        <v>-170.10086418676</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -749,17 +788,20 @@
       <c r="D16" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="E16" s="1" t="n">
+        <v>0.1</v>
+      </c>
       <c r="F16" s="2" t="n">
-        <f aca="false">$E$2/(1-(1/(1+$E$2)^C16))</f>
-        <v>0.0888274333872723</v>
+        <f aca="false">E16/(1-(1/(1+E16)^C16))</f>
+        <v>0.106079248252634</v>
       </c>
       <c r="G16" s="2" t="n">
         <f aca="false">F16/(1-(1/(1+F16)^D16))</f>
-        <v>0.155016799199575</v>
+        <v>0.167019608595705</v>
       </c>
       <c r="I16" s="3" t="n">
         <f aca="false">B16/(1-$H$2)*F16/G16</f>
-        <v>-69.447387494249</v>
+        <v>-76.9751486618614</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -775,17 +817,20 @@
       <c r="D17" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="E17" s="1" t="n">
+        <v>0.1</v>
+      </c>
       <c r="F17" s="2" t="n">
-        <f aca="false">$E$2/(1-(1/(1+$E$2)^C17))</f>
-        <v>0.0888274333872723</v>
+        <f aca="false">E17/(1-(1/(1+E17)^C17))</f>
+        <v>0.106079248252634</v>
       </c>
       <c r="G17" s="2" t="n">
         <f aca="false">F17/(1-(1/(1+F17)^D17))</f>
-        <v>0.155016799199575</v>
+        <v>0.167019608595705</v>
       </c>
       <c r="I17" s="3" t="n">
         <f aca="false">B17/(1-$H$2)*F17/G17</f>
-        <v>-69.447387494249</v>
+        <v>-76.9751486618614</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -801,17 +846,20 @@
       <c r="D18" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="E18" s="1" t="n">
+        <v>0.1</v>
+      </c>
       <c r="F18" s="2" t="n">
-        <f aca="false">$E$2/(1-(1/(1+$E$2)^C18))</f>
-        <v>0.0888274333872723</v>
+        <f aca="false">E18/(1-(1/(1+E18)^C18))</f>
+        <v>0.106079248252634</v>
       </c>
       <c r="G18" s="2" t="n">
         <f aca="false">F18/(1-(1/(1+F18)^D18))</f>
-        <v>0.155016799199575</v>
+        <v>0.167019608595705</v>
       </c>
       <c r="I18" s="3" t="n">
         <f aca="false">B18/(1-$H$2)*F18/G18</f>
-        <v>-69.447387494249</v>
+        <v>-76.9751486618614</v>
       </c>
     </row>
   </sheetData>
@@ -881,22 +929,22 @@
         <v>10</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>0.08</v>
+        <v>0.07</v>
       </c>
       <c r="F2" s="2" t="n">
         <f aca="false">$E$2/(1-(1/(1+$E$2)^C2))</f>
-        <v>0.101852208823151</v>
+        <v>0.0943929257432557</v>
       </c>
       <c r="G2" s="2" t="n">
         <f aca="false">F2/(1-(1/(1+F2)^D2))</f>
-        <v>0.164042574503865</v>
+        <v>0.158845968886606</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>0.2574</v>
       </c>
       <c r="I2" s="3" t="n">
         <f aca="false">B2/(1-$H$2)*F2/G2</f>
-        <v>-25.083040829073</v>
+        <v>-24.0065393594822</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix units for tax credits
</commit_message>
<xml_diff>
--- a/data/tax_credits/tax_credits_calculations.xlsx
+++ b/data/tax_credits/tax_credits_calculations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="production_tax_credits" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t xml:space="preserve">carrier</t>
   </si>
@@ -35,7 +35,7 @@
     <t xml:space="preserve">credit lifetime (years)</t>
   </si>
   <si>
-    <t xml:space="preserve">discount rate</t>
+    <t xml:space="preserve">discount rate (-)</t>
   </si>
   <si>
     <t xml:space="preserve">CRF (-)</t>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t xml:space="preserve">SOEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax credit (% inv. cost)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">levelized tax credit (% inv. cost)</t>
   </si>
   <si>
     <t xml:space="preserve">battery</t>
@@ -320,8 +326,8 @@
   </sheetPr>
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -880,8 +886,8 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -891,7 +897,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -912,12 +918,12 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>-30</v>

</xml_diff>

<commit_message>
Update tax credit values based on actual discount rates
</commit_message>
<xml_diff>
--- a/data/tax_credits/tax_credits_calculations.xlsx
+++ b/data/tax_credits/tax_credits_calculations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="production_tax_credits" sheetId="1" state="visible" r:id="rId3"/>
@@ -184,12 +184,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -326,8 +330,8 @@
   </sheetPr>
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -385,23 +389,23 @@
       <c r="D2" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="F2" s="2" t="n">
+      <c r="E2" s="2" t="n">
+        <v>0.0320752195121951</v>
+      </c>
+      <c r="F2" s="3" t="n">
         <f aca="false">E2/(1-(1/(1+E2)^C2))</f>
-        <v>0.0712292255000195</v>
-      </c>
-      <c r="G2" s="2" t="n">
+        <v>0.0377544133129132</v>
+      </c>
+      <c r="G2" s="3" t="n">
         <f aca="false">F2/(1-(1/(1+F2)^D2))</f>
-        <v>0.154290036689704</v>
+        <v>0.133120250116782</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>0.2574</v>
       </c>
-      <c r="I2" s="3" t="n">
+      <c r="I2" s="4" t="n">
         <f aca="false">B2/(1-$H$2)*F2/G2</f>
-        <v>-9.32516777004039</v>
+        <v>-5.72875059212375</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -417,20 +421,20 @@
       <c r="D3" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="F3" s="2" t="n">
+      <c r="E3" s="2" t="n">
+        <v>0.0564730561021376</v>
+      </c>
+      <c r="F3" s="3" t="n">
         <f aca="false">E3/(1-(1/(1+E3)^C3))</f>
-        <v>0.0712292255000195</v>
-      </c>
-      <c r="G3" s="2" t="n">
+        <v>0.058644360583871</v>
+      </c>
+      <c r="G3" s="3" t="n">
         <f aca="false">F3/(1-(1/(1+F3)^D3))</f>
-        <v>0.143187579596091</v>
-      </c>
-      <c r="I3" s="3" t="n">
+        <v>0.134996667773367</v>
+      </c>
+      <c r="I3" s="4" t="n">
         <f aca="false">B3/(1-$H$2)*F3/G3</f>
-        <v>-18.4217389243225</v>
+        <v>-16.0872183226418</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -446,20 +450,20 @@
       <c r="D4" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E4" s="1" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="F4" s="2" t="n">
+      <c r="E4" s="2" t="n">
+        <v>0.051519516365778</v>
+      </c>
+      <c r="F4" s="3" t="n">
         <f aca="false">E4/(1-(1/(1+E4)^C4))</f>
-        <v>0.0805864035111112</v>
-      </c>
-      <c r="G4" s="2" t="n">
+        <v>0.0661825298559019</v>
+      </c>
+      <c r="G4" s="3" t="n">
         <f aca="false">F4/(1-(1/(1+F4)^D4))</f>
-        <v>0.149423903774895</v>
-      </c>
-      <c r="I4" s="3" t="n">
+        <v>0.139875489551139</v>
+      </c>
+      <c r="I4" s="4" t="n">
         <f aca="false">B4/(1-$H$2)*F4/G4</f>
-        <v>-19.9719028411147</v>
+        <v>-17.5218312601058</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -475,20 +479,20 @@
       <c r="D5" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E5" s="1" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="F5" s="2" t="n">
+      <c r="E5" s="2" t="n">
+        <v>0.0538314857296738</v>
+      </c>
+      <c r="F5" s="3" t="n">
         <f aca="false">E5/(1-(1/(1+E5)^C5))</f>
-        <v>0.0805864035111112</v>
-      </c>
-      <c r="G5" s="2" t="n">
+        <v>0.0679198927879237</v>
+      </c>
+      <c r="G5" s="3" t="n">
         <f aca="false">F5/(1-(1/(1+F5)^D5))</f>
-        <v>0.149423903774895</v>
-      </c>
-      <c r="I5" s="3" t="n">
+        <v>0.141011589512446</v>
+      </c>
+      <c r="I5" s="4" t="n">
         <f aca="false">B5/(1-$H$2)*F5/G5</f>
-        <v>-19.9719028411147</v>
+        <v>-17.8369227964236</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -504,20 +508,20 @@
       <c r="D6" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E6" s="1" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="F6" s="2" t="n">
+      <c r="E6" s="2" t="n">
+        <v>0.0438437157985803</v>
+      </c>
+      <c r="F6" s="3" t="n">
         <f aca="false">E6/(1-(1/(1+E6)^C6))</f>
-        <v>0.0772339596490032</v>
-      </c>
-      <c r="G6" s="2" t="n">
+        <v>0.0564065527786497</v>
+      </c>
+      <c r="G6" s="3" t="n">
         <f aca="false">F6/(1-(1/(1+F6)^D6))</f>
-        <v>0.147175489847447</v>
-      </c>
-      <c r="I6" s="3" t="n">
+        <v>0.133564295407616</v>
+      </c>
+      <c r="I6" s="4" t="n">
         <f aca="false">B6/(1-$H$2)*F6/G6</f>
-        <v>-19.4334792027051</v>
+        <v>-15.6392863181404</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -533,20 +537,20 @@
       <c r="D7" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E7" s="1" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="F7" s="2" t="n">
+      <c r="E7" s="2" t="n">
+        <v>0.0519007613262936</v>
+      </c>
+      <c r="F7" s="3" t="n">
         <f aca="false">E7/(1-(1/(1+E7)^C7))</f>
-        <v>0.0834257340177891</v>
-      </c>
-      <c r="G7" s="2" t="n">
+        <v>0.0696731977196162</v>
+      </c>
+      <c r="G7" s="3" t="n">
         <f aca="false">F7/(1-(1/(1+F7)^D7))</f>
-        <v>0.151340354350156</v>
-      </c>
-      <c r="I7" s="3" t="n">
+        <v>0.142162497334978</v>
+      </c>
+      <c r="I7" s="4" t="n">
         <f aca="false">B7/(1-$H$2)*F7/G7</f>
-        <v>-20.4137616145153</v>
+        <v>-18.1492401935753</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -562,20 +566,20 @@
       <c r="D8" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E8" s="1" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="F8" s="2" t="n">
+      <c r="E8" s="2" t="n">
+        <v>0.0515227657596506</v>
+      </c>
+      <c r="F8" s="3" t="n">
         <f aca="false">E8/(1-(1/(1+E8)^C8))</f>
-        <v>0.0834257340177891</v>
-      </c>
-      <c r="G8" s="2" t="n">
+        <v>0.0693974933274804</v>
+      </c>
+      <c r="G8" s="3" t="n">
         <f aca="false">F8/(1-(1/(1+F8)^D8))</f>
-        <v>0.151340354350156</v>
-      </c>
-      <c r="I8" s="3" t="n">
+        <v>0.141981227994836</v>
+      </c>
+      <c r="I8" s="4" t="n">
         <f aca="false">B8/(1-$H$2)*F8/G8</f>
-        <v>-20.4137616145153</v>
+        <v>-18.100501370732</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -591,20 +595,20 @@
       <c r="D9" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E9" s="1" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="F9" s="2" t="n">
+      <c r="E9" s="2" t="n">
+        <v>0.0515227657596506</v>
+      </c>
+      <c r="F9" s="3" t="n">
         <f aca="false">E9/(1-(1/(1+E9)^C9))</f>
-        <v>0.0834257340177891</v>
-      </c>
-      <c r="G9" s="2" t="n">
+        <v>0.0693974933274804</v>
+      </c>
+      <c r="G9" s="3" t="n">
         <f aca="false">F9/(1-(1/(1+F9)^D9))</f>
-        <v>0.151340354350156</v>
-      </c>
-      <c r="I9" s="3" t="n">
+        <v>0.141981227994836</v>
+      </c>
+      <c r="I9" s="4" t="n">
         <f aca="false">B9/(1-$H$2)*F9/G9</f>
-        <v>-20.4137616145153</v>
+        <v>-18.100501370732</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -620,18 +624,18 @@
       <c r="D10" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="3" t="n">
         <v>0.07</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="3" t="n">
         <f aca="false">E10/(1-(1/(1+E10)^C10))</f>
         <v>0.0943929257432557</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G10" s="3" t="n">
         <f aca="false">F10/(1-(1/(1+F10)^D10))</f>
         <v>0.142756193054826</v>
       </c>
-      <c r="I10" s="3" t="n">
+      <c r="I10" s="4" t="n">
         <f aca="false">B10/(1-$H$2)*F10/G10</f>
         <v>-75.6847656176249</v>
       </c>
@@ -649,18 +653,18 @@
       <c r="D11" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="3" t="n">
         <v>0.07</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="3" t="n">
         <f aca="false">E11/(1-(1/(1+E11)^C11))</f>
         <v>0.0943929257432557</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G11" s="3" t="n">
         <f aca="false">F11/(1-(1/(1+F11)^D11))</f>
         <v>0.142756193054826</v>
       </c>
-      <c r="I11" s="3" t="n">
+      <c r="I11" s="4" t="n">
         <f aca="false">B11/(1-$H$2)*F11/G11</f>
         <v>-75.6847656176249</v>
       </c>
@@ -678,18 +682,18 @@
       <c r="D12" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="3" t="n">
         <v>0.07</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="3" t="n">
         <f aca="false">E12/(1-(1/(1+E12)^C12))</f>
         <v>0.0943929257432557</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="G12" s="3" t="n">
         <f aca="false">F12/(1-(1/(1+F12)^D12))</f>
         <v>0.142756193054826</v>
       </c>
-      <c r="I12" s="3" t="n">
+      <c r="I12" s="4" t="n">
         <f aca="false">B12/(1-$H$2)*F12/G12</f>
         <v>-75.6847656176249</v>
       </c>
@@ -707,18 +711,18 @@
       <c r="D13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="3" t="n">
         <v>0.07</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F13" s="3" t="n">
         <f aca="false">E13/(1-(1/(1+E13)^C13))</f>
         <v>0.0943929257432557</v>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="G13" s="3" t="n">
         <f aca="false">F13/(1-(1/(1+F13)^D13))</f>
         <v>0.142756193054826</v>
       </c>
-      <c r="I13" s="3" t="n">
+      <c r="I13" s="4" t="n">
         <f aca="false">B13/(1-$H$2)*F13/G13</f>
         <v>-75.6847656176249</v>
       </c>
@@ -736,18 +740,18 @@
       <c r="D14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="3" t="n">
         <v>0.07</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="3" t="n">
         <f aca="false">E14/(1-(1/(1+E14)^C14))</f>
         <v>0.0943929257432557</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="G14" s="3" t="n">
         <f aca="false">F14/(1-(1/(1+F14)^D14))</f>
         <v>0.142756193054826</v>
       </c>
-      <c r="I14" s="3" t="n">
+      <c r="I14" s="4" t="n">
         <f aca="false">B14/(1-$H$2)*F14/G14</f>
         <v>-75.6847656176249</v>
       </c>
@@ -765,18 +769,18 @@
       <c r="D15" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="3" t="n">
         <v>0.1</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F15" s="3" t="n">
         <f aca="false">E15/(1-(1/(1+E15)^C15))</f>
         <v>0.106079248252634</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G15" s="3" t="n">
         <f aca="false">F15/(1-(1/(1+F15)^D15))</f>
         <v>0.151161597709284</v>
       </c>
-      <c r="I15" s="3" t="n">
+      <c r="I15" s="4" t="n">
         <f aca="false">B15/(1-$H$2)*F15/G15</f>
         <v>-170.10086418676</v>
       </c>
@@ -794,18 +798,18 @@
       <c r="D16" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E16" s="1" t="n">
+      <c r="E16" s="3" t="n">
         <v>0.1</v>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F16" s="3" t="n">
         <f aca="false">E16/(1-(1/(1+E16)^C16))</f>
         <v>0.106079248252634</v>
       </c>
-      <c r="G16" s="2" t="n">
+      <c r="G16" s="3" t="n">
         <f aca="false">F16/(1-(1/(1+F16)^D16))</f>
         <v>0.167019608595705</v>
       </c>
-      <c r="I16" s="3" t="n">
+      <c r="I16" s="4" t="n">
         <f aca="false">B16/(1-$H$2)*F16/G16</f>
         <v>-76.9751486618614</v>
       </c>
@@ -823,18 +827,18 @@
       <c r="D17" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E17" s="1" t="n">
+      <c r="E17" s="3" t="n">
         <v>0.1</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F17" s="3" t="n">
         <f aca="false">E17/(1-(1/(1+E17)^C17))</f>
         <v>0.106079248252634</v>
       </c>
-      <c r="G17" s="2" t="n">
+      <c r="G17" s="3" t="n">
         <f aca="false">F17/(1-(1/(1+F17)^D17))</f>
         <v>0.167019608595705</v>
       </c>
-      <c r="I17" s="3" t="n">
+      <c r="I17" s="4" t="n">
         <f aca="false">B17/(1-$H$2)*F17/G17</f>
         <v>-76.9751486618614</v>
       </c>
@@ -852,18 +856,18 @@
       <c r="D18" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="E18" s="3" t="n">
         <v>0.1</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F18" s="3" t="n">
         <f aca="false">E18/(1-(1/(1+E18)^C18))</f>
         <v>0.106079248252634</v>
       </c>
-      <c r="G18" s="2" t="n">
+      <c r="G18" s="3" t="n">
         <f aca="false">F18/(1-(1/(1+F18)^D18))</f>
         <v>0.167019608595705</v>
       </c>
-      <c r="I18" s="3" t="n">
+      <c r="I18" s="4" t="n">
         <f aca="false">B18/(1-$H$2)*F18/G18</f>
         <v>-76.9751486618614</v>
       </c>
@@ -886,8 +890,8 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -937,18 +941,18 @@
       <c r="E2" s="1" t="n">
         <v>0.07</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="3" t="n">
         <f aca="false">$E$2/(1-(1/(1+$E$2)^C2))</f>
         <v>0.0943929257432557</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="3" t="n">
         <f aca="false">F2/(1-(1/(1+F2)^D2))</f>
         <v>0.158845968886606</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>0.2574</v>
       </c>
-      <c r="I2" s="3" t="n">
+      <c r="I2" s="4" t="n">
         <f aca="false">B2/(1-$H$2)*F2/G2</f>
         <v>-24.0065393594822</v>
       </c>

</xml_diff>

<commit_message>
Update tax credit values based on actual discount rates (#116)
* Update tax credit values based on actual discount rates

* Approximate tax credit values

* update release notes
</commit_message>
<xml_diff>
--- a/data/tax_credits/tax_credits_calculations.xlsx
+++ b/data/tax_credits/tax_credits_calculations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="production_tax_credits" sheetId="1" state="visible" r:id="rId3"/>
@@ -184,12 +184,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -326,8 +330,8 @@
   </sheetPr>
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -385,23 +389,23 @@
       <c r="D2" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="F2" s="2" t="n">
+      <c r="E2" s="2" t="n">
+        <v>0.0320752195121951</v>
+      </c>
+      <c r="F2" s="3" t="n">
         <f aca="false">E2/(1-(1/(1+E2)^C2))</f>
-        <v>0.0712292255000195</v>
-      </c>
-      <c r="G2" s="2" t="n">
+        <v>0.0377544133129132</v>
+      </c>
+      <c r="G2" s="3" t="n">
         <f aca="false">F2/(1-(1/(1+F2)^D2))</f>
-        <v>0.154290036689704</v>
+        <v>0.133120250116782</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>0.2574</v>
       </c>
-      <c r="I2" s="3" t="n">
+      <c r="I2" s="4" t="n">
         <f aca="false">B2/(1-$H$2)*F2/G2</f>
-        <v>-9.32516777004039</v>
+        <v>-5.72875059212375</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -417,20 +421,20 @@
       <c r="D3" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="F3" s="2" t="n">
+      <c r="E3" s="2" t="n">
+        <v>0.0564730561021376</v>
+      </c>
+      <c r="F3" s="3" t="n">
         <f aca="false">E3/(1-(1/(1+E3)^C3))</f>
-        <v>0.0712292255000195</v>
-      </c>
-      <c r="G3" s="2" t="n">
+        <v>0.058644360583871</v>
+      </c>
+      <c r="G3" s="3" t="n">
         <f aca="false">F3/(1-(1/(1+F3)^D3))</f>
-        <v>0.143187579596091</v>
-      </c>
-      <c r="I3" s="3" t="n">
+        <v>0.134996667773367</v>
+      </c>
+      <c r="I3" s="4" t="n">
         <f aca="false">B3/(1-$H$2)*F3/G3</f>
-        <v>-18.4217389243225</v>
+        <v>-16.0872183226418</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -446,20 +450,20 @@
       <c r="D4" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E4" s="1" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="F4" s="2" t="n">
+      <c r="E4" s="2" t="n">
+        <v>0.051519516365778</v>
+      </c>
+      <c r="F4" s="3" t="n">
         <f aca="false">E4/(1-(1/(1+E4)^C4))</f>
-        <v>0.0805864035111112</v>
-      </c>
-      <c r="G4" s="2" t="n">
+        <v>0.0661825298559019</v>
+      </c>
+      <c r="G4" s="3" t="n">
         <f aca="false">F4/(1-(1/(1+F4)^D4))</f>
-        <v>0.149423903774895</v>
-      </c>
-      <c r="I4" s="3" t="n">
+        <v>0.139875489551139</v>
+      </c>
+      <c r="I4" s="4" t="n">
         <f aca="false">B4/(1-$H$2)*F4/G4</f>
-        <v>-19.9719028411147</v>
+        <v>-17.5218312601058</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -475,20 +479,20 @@
       <c r="D5" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E5" s="1" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="F5" s="2" t="n">
+      <c r="E5" s="2" t="n">
+        <v>0.0538314857296738</v>
+      </c>
+      <c r="F5" s="3" t="n">
         <f aca="false">E5/(1-(1/(1+E5)^C5))</f>
-        <v>0.0805864035111112</v>
-      </c>
-      <c r="G5" s="2" t="n">
+        <v>0.0679198927879237</v>
+      </c>
+      <c r="G5" s="3" t="n">
         <f aca="false">F5/(1-(1/(1+F5)^D5))</f>
-        <v>0.149423903774895</v>
-      </c>
-      <c r="I5" s="3" t="n">
+        <v>0.141011589512446</v>
+      </c>
+      <c r="I5" s="4" t="n">
         <f aca="false">B5/(1-$H$2)*F5/G5</f>
-        <v>-19.9719028411147</v>
+        <v>-17.8369227964236</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -504,20 +508,20 @@
       <c r="D6" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E6" s="1" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="F6" s="2" t="n">
+      <c r="E6" s="2" t="n">
+        <v>0.0438437157985803</v>
+      </c>
+      <c r="F6" s="3" t="n">
         <f aca="false">E6/(1-(1/(1+E6)^C6))</f>
-        <v>0.0772339596490032</v>
-      </c>
-      <c r="G6" s="2" t="n">
+        <v>0.0564065527786497</v>
+      </c>
+      <c r="G6" s="3" t="n">
         <f aca="false">F6/(1-(1/(1+F6)^D6))</f>
-        <v>0.147175489847447</v>
-      </c>
-      <c r="I6" s="3" t="n">
+        <v>0.133564295407616</v>
+      </c>
+      <c r="I6" s="4" t="n">
         <f aca="false">B6/(1-$H$2)*F6/G6</f>
-        <v>-19.4334792027051</v>
+        <v>-15.6392863181404</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -533,20 +537,20 @@
       <c r="D7" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E7" s="1" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="F7" s="2" t="n">
+      <c r="E7" s="2" t="n">
+        <v>0.0519007613262936</v>
+      </c>
+      <c r="F7" s="3" t="n">
         <f aca="false">E7/(1-(1/(1+E7)^C7))</f>
-        <v>0.0834257340177891</v>
-      </c>
-      <c r="G7" s="2" t="n">
+        <v>0.0696731977196162</v>
+      </c>
+      <c r="G7" s="3" t="n">
         <f aca="false">F7/(1-(1/(1+F7)^D7))</f>
-        <v>0.151340354350156</v>
-      </c>
-      <c r="I7" s="3" t="n">
+        <v>0.142162497334978</v>
+      </c>
+      <c r="I7" s="4" t="n">
         <f aca="false">B7/(1-$H$2)*F7/G7</f>
-        <v>-20.4137616145153</v>
+        <v>-18.1492401935753</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -562,20 +566,20 @@
       <c r="D8" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E8" s="1" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="F8" s="2" t="n">
+      <c r="E8" s="2" t="n">
+        <v>0.0515227657596506</v>
+      </c>
+      <c r="F8" s="3" t="n">
         <f aca="false">E8/(1-(1/(1+E8)^C8))</f>
-        <v>0.0834257340177891</v>
-      </c>
-      <c r="G8" s="2" t="n">
+        <v>0.0693974933274804</v>
+      </c>
+      <c r="G8" s="3" t="n">
         <f aca="false">F8/(1-(1/(1+F8)^D8))</f>
-        <v>0.151340354350156</v>
-      </c>
-      <c r="I8" s="3" t="n">
+        <v>0.141981227994836</v>
+      </c>
+      <c r="I8" s="4" t="n">
         <f aca="false">B8/(1-$H$2)*F8/G8</f>
-        <v>-20.4137616145153</v>
+        <v>-18.100501370732</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -591,20 +595,20 @@
       <c r="D9" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E9" s="1" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="F9" s="2" t="n">
+      <c r="E9" s="2" t="n">
+        <v>0.0515227657596506</v>
+      </c>
+      <c r="F9" s="3" t="n">
         <f aca="false">E9/(1-(1/(1+E9)^C9))</f>
-        <v>0.0834257340177891</v>
-      </c>
-      <c r="G9" s="2" t="n">
+        <v>0.0693974933274804</v>
+      </c>
+      <c r="G9" s="3" t="n">
         <f aca="false">F9/(1-(1/(1+F9)^D9))</f>
-        <v>0.151340354350156</v>
-      </c>
-      <c r="I9" s="3" t="n">
+        <v>0.141981227994836</v>
+      </c>
+      <c r="I9" s="4" t="n">
         <f aca="false">B9/(1-$H$2)*F9/G9</f>
-        <v>-20.4137616145153</v>
+        <v>-18.100501370732</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -620,18 +624,18 @@
       <c r="D10" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="3" t="n">
         <v>0.07</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="3" t="n">
         <f aca="false">E10/(1-(1/(1+E10)^C10))</f>
         <v>0.0943929257432557</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G10" s="3" t="n">
         <f aca="false">F10/(1-(1/(1+F10)^D10))</f>
         <v>0.142756193054826</v>
       </c>
-      <c r="I10" s="3" t="n">
+      <c r="I10" s="4" t="n">
         <f aca="false">B10/(1-$H$2)*F10/G10</f>
         <v>-75.6847656176249</v>
       </c>
@@ -649,18 +653,18 @@
       <c r="D11" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="3" t="n">
         <v>0.07</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="3" t="n">
         <f aca="false">E11/(1-(1/(1+E11)^C11))</f>
         <v>0.0943929257432557</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G11" s="3" t="n">
         <f aca="false">F11/(1-(1/(1+F11)^D11))</f>
         <v>0.142756193054826</v>
       </c>
-      <c r="I11" s="3" t="n">
+      <c r="I11" s="4" t="n">
         <f aca="false">B11/(1-$H$2)*F11/G11</f>
         <v>-75.6847656176249</v>
       </c>
@@ -678,18 +682,18 @@
       <c r="D12" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="3" t="n">
         <v>0.07</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="3" t="n">
         <f aca="false">E12/(1-(1/(1+E12)^C12))</f>
         <v>0.0943929257432557</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="G12" s="3" t="n">
         <f aca="false">F12/(1-(1/(1+F12)^D12))</f>
         <v>0.142756193054826</v>
       </c>
-      <c r="I12" s="3" t="n">
+      <c r="I12" s="4" t="n">
         <f aca="false">B12/(1-$H$2)*F12/G12</f>
         <v>-75.6847656176249</v>
       </c>
@@ -707,18 +711,18 @@
       <c r="D13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="3" t="n">
         <v>0.07</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F13" s="3" t="n">
         <f aca="false">E13/(1-(1/(1+E13)^C13))</f>
         <v>0.0943929257432557</v>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="G13" s="3" t="n">
         <f aca="false">F13/(1-(1/(1+F13)^D13))</f>
         <v>0.142756193054826</v>
       </c>
-      <c r="I13" s="3" t="n">
+      <c r="I13" s="4" t="n">
         <f aca="false">B13/(1-$H$2)*F13/G13</f>
         <v>-75.6847656176249</v>
       </c>
@@ -736,18 +740,18 @@
       <c r="D14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="3" t="n">
         <v>0.07</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="3" t="n">
         <f aca="false">E14/(1-(1/(1+E14)^C14))</f>
         <v>0.0943929257432557</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="G14" s="3" t="n">
         <f aca="false">F14/(1-(1/(1+F14)^D14))</f>
         <v>0.142756193054826</v>
       </c>
-      <c r="I14" s="3" t="n">
+      <c r="I14" s="4" t="n">
         <f aca="false">B14/(1-$H$2)*F14/G14</f>
         <v>-75.6847656176249</v>
       </c>
@@ -765,18 +769,18 @@
       <c r="D15" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="3" t="n">
         <v>0.1</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F15" s="3" t="n">
         <f aca="false">E15/(1-(1/(1+E15)^C15))</f>
         <v>0.106079248252634</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G15" s="3" t="n">
         <f aca="false">F15/(1-(1/(1+F15)^D15))</f>
         <v>0.151161597709284</v>
       </c>
-      <c r="I15" s="3" t="n">
+      <c r="I15" s="4" t="n">
         <f aca="false">B15/(1-$H$2)*F15/G15</f>
         <v>-170.10086418676</v>
       </c>
@@ -794,18 +798,18 @@
       <c r="D16" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E16" s="1" t="n">
+      <c r="E16" s="3" t="n">
         <v>0.1</v>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F16" s="3" t="n">
         <f aca="false">E16/(1-(1/(1+E16)^C16))</f>
         <v>0.106079248252634</v>
       </c>
-      <c r="G16" s="2" t="n">
+      <c r="G16" s="3" t="n">
         <f aca="false">F16/(1-(1/(1+F16)^D16))</f>
         <v>0.167019608595705</v>
       </c>
-      <c r="I16" s="3" t="n">
+      <c r="I16" s="4" t="n">
         <f aca="false">B16/(1-$H$2)*F16/G16</f>
         <v>-76.9751486618614</v>
       </c>
@@ -823,18 +827,18 @@
       <c r="D17" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E17" s="1" t="n">
+      <c r="E17" s="3" t="n">
         <v>0.1</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F17" s="3" t="n">
         <f aca="false">E17/(1-(1/(1+E17)^C17))</f>
         <v>0.106079248252634</v>
       </c>
-      <c r="G17" s="2" t="n">
+      <c r="G17" s="3" t="n">
         <f aca="false">F17/(1-(1/(1+F17)^D17))</f>
         <v>0.167019608595705</v>
       </c>
-      <c r="I17" s="3" t="n">
+      <c r="I17" s="4" t="n">
         <f aca="false">B17/(1-$H$2)*F17/G17</f>
         <v>-76.9751486618614</v>
       </c>
@@ -852,18 +856,18 @@
       <c r="D18" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="E18" s="3" t="n">
         <v>0.1</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F18" s="3" t="n">
         <f aca="false">E18/(1-(1/(1+E18)^C18))</f>
         <v>0.106079248252634</v>
       </c>
-      <c r="G18" s="2" t="n">
+      <c r="G18" s="3" t="n">
         <f aca="false">F18/(1-(1/(1+F18)^D18))</f>
         <v>0.167019608595705</v>
       </c>
-      <c r="I18" s="3" t="n">
+      <c r="I18" s="4" t="n">
         <f aca="false">B18/(1-$H$2)*F18/G18</f>
         <v>-76.9751486618614</v>
       </c>
@@ -886,8 +890,8 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -937,18 +941,18 @@
       <c r="E2" s="1" t="n">
         <v>0.07</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="3" t="n">
         <f aca="false">$E$2/(1-(1/(1+$E$2)^C2))</f>
         <v>0.0943929257432557</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="3" t="n">
         <f aca="false">F2/(1-(1/(1+F2)^D2))</f>
         <v>0.158845968886606</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>0.2574</v>
       </c>
-      <c r="I2" s="3" t="n">
+      <c r="I2" s="4" t="n">
         <f aca="false">B2/(1-$H$2)*F2/G2</f>
         <v>-24.0065393594822</v>
       </c>

</xml_diff>

<commit_message>
apply usage-only 45Q credits for CC and DAC, unify credit logic across regimes and update eligible CO2 bus detection
</commit_message>
<xml_diff>
--- a/data/tax_credits/tax_credits_calculations.xlsx
+++ b/data/tax_credits/tax_credits_calculations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="production_tax_credits" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t xml:space="preserve">carrier</t>
   </si>
@@ -50,6 +50,9 @@
     <t xml:space="preserve">levelized tax credit ($/output unit)</t>
   </si>
   <si>
+    <t xml:space="preserve">regime</t>
+  </si>
+  <si>
     <t xml:space="preserve">nuclear_existing</t>
   </si>
   <si>
@@ -77,6 +80,9 @@
     <t xml:space="preserve">ethanol from starch CC</t>
   </si>
   <si>
+    <t xml:space="preserve">OB3</t>
+  </si>
+  <si>
     <t xml:space="preserve">SMR CC</t>
   </si>
   <si>
@@ -90,6 +96,9 @@
   </si>
   <si>
     <t xml:space="preserve">DAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRA 2022</t>
   </si>
   <si>
     <t xml:space="preserve">Alkaline electrolyzer large</t>
@@ -193,7 +202,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -328,10 +337,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J21" activeCellId="0" sqref="I10:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -375,10 +384,13 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>-15</v>
@@ -389,7 +401,7 @@
       <c r="D2" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="3" t="n">
         <v>0.0320752195121951</v>
       </c>
       <c r="F2" s="3" t="n">
@@ -410,7 +422,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>-27.5</v>
@@ -421,7 +433,7 @@
       <c r="D3" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="3" t="n">
         <v>0.0564730561021376</v>
       </c>
       <c r="F3" s="3" t="n">
@@ -439,7 +451,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>-27.5</v>
@@ -450,7 +462,7 @@
       <c r="D4" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="3" t="n">
         <v>0.051519516365778</v>
       </c>
       <c r="F4" s="3" t="n">
@@ -468,7 +480,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>-27.5</v>
@@ -479,7 +491,7 @@
       <c r="D5" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="3" t="n">
         <v>0.0538314857296738</v>
       </c>
       <c r="F5" s="3" t="n">
@@ -497,7 +509,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>-27.5</v>
@@ -508,7 +520,7 @@
       <c r="D6" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="3" t="n">
         <v>0.0438437157985803</v>
       </c>
       <c r="F6" s="3" t="n">
@@ -526,7 +538,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>-27.5</v>
@@ -537,7 +549,7 @@
       <c r="D7" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="3" t="n">
         <v>0.0519007613262936</v>
       </c>
       <c r="F7" s="3" t="n">
@@ -555,7 +567,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>-27.5</v>
@@ -566,7 +578,7 @@
       <c r="D8" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="3" t="n">
         <v>0.0515227657596506</v>
       </c>
       <c r="F8" s="3" t="n">
@@ -584,7 +596,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>-27.5</v>
@@ -595,7 +607,7 @@
       <c r="D9" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E9" s="2" t="n">
+      <c r="E9" s="3" t="n">
         <v>0.0515227657596506</v>
       </c>
       <c r="F9" s="3" t="n">
@@ -613,7 +625,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>-85</v>
@@ -639,10 +651,13 @@
         <f aca="false">B10/(1-$H$2)*F10/G10</f>
         <v>-75.6847656176249</v>
       </c>
+      <c r="J10" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>-85</v>
@@ -668,10 +683,13 @@
         <f aca="false">B11/(1-$H$2)*F11/G11</f>
         <v>-75.6847656176249</v>
       </c>
+      <c r="J11" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>-85</v>
@@ -697,10 +715,13 @@
         <f aca="false">B12/(1-$H$2)*F12/G12</f>
         <v>-75.6847656176249</v>
       </c>
+      <c r="J12" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>-85</v>
@@ -726,10 +747,13 @@
         <f aca="false">B13/(1-$H$2)*F13/G13</f>
         <v>-75.6847656176249</v>
       </c>
+      <c r="J13" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>-85</v>
@@ -755,10 +779,13 @@
         <f aca="false">B14/(1-$H$2)*F14/G14</f>
         <v>-75.6847656176249</v>
       </c>
+      <c r="J14" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>-180</v>
@@ -784,91 +811,286 @@
         <f aca="false">B15/(1-$H$2)*F15/G15</f>
         <v>-170.10086418676</v>
       </c>
+      <c r="J15" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>-90</v>
+        <v>-60</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>0.1</v>
+        <v>0.07</v>
       </c>
       <c r="F16" s="3" t="n">
         <f aca="false">E16/(1-(1/(1+E16)^C16))</f>
-        <v>0.106079248252634</v>
+        <v>0.0943929257432557</v>
       </c>
       <c r="G16" s="3" t="n">
         <f aca="false">F16/(1-(1/(1+F16)^D16))</f>
-        <v>0.167019608595705</v>
+        <v>0.142756193054826</v>
       </c>
       <c r="I16" s="4" t="n">
         <f aca="false">B16/(1-$H$2)*F16/G16</f>
-        <v>-76.9751486618614</v>
+        <v>-53.4245404359705</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>-90</v>
+        <v>-60</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>0.1</v>
+        <v>0.07</v>
       </c>
       <c r="F17" s="3" t="n">
         <f aca="false">E17/(1-(1/(1+E17)^C17))</f>
-        <v>0.106079248252634</v>
+        <v>0.0943929257432557</v>
       </c>
       <c r="G17" s="3" t="n">
         <f aca="false">F17/(1-(1/(1+F17)^D17))</f>
-        <v>0.167019608595705</v>
+        <v>0.142756193054826</v>
       </c>
       <c r="I17" s="4" t="n">
         <f aca="false">B17/(1-$H$2)*F17/G17</f>
-        <v>-76.9751486618614</v>
+        <v>-53.4245404359705</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>-90</v>
+        <v>-60</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>0.1</v>
+        <v>0.07</v>
       </c>
       <c r="F18" s="3" t="n">
         <f aca="false">E18/(1-(1/(1+E18)^C18))</f>
-        <v>0.106079248252634</v>
+        <v>0.0943929257432557</v>
       </c>
       <c r="G18" s="3" t="n">
         <f aca="false">F18/(1-(1/(1+F18)^D18))</f>
-        <v>0.167019608595705</v>
+        <v>0.142756193054826</v>
       </c>
       <c r="I18" s="4" t="n">
         <f aca="false">B18/(1-$H$2)*F18/G18</f>
+        <v>-53.4245404359705</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <f aca="false">E19/(1-(1/(1+E19)^C19))</f>
+        <v>0.0943929257432557</v>
+      </c>
+      <c r="G19" s="3" t="n">
+        <f aca="false">F19/(1-(1/(1+F19)^D19))</f>
+        <v>0.142756193054826</v>
+      </c>
+      <c r="I19" s="4" t="n">
+        <f aca="false">B19/(1-$H$2)*F19/G19</f>
+        <v>-53.4245404359705</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="E20" s="3" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="F20" s="3" t="n">
+        <f aca="false">E20/(1-(1/(1+E20)^C20))</f>
+        <v>0.0943929257432557</v>
+      </c>
+      <c r="G20" s="3" t="n">
+        <f aca="false">F20/(1-(1/(1+F20)^D20))</f>
+        <v>0.142756193054826</v>
+      </c>
+      <c r="I20" s="4" t="n">
+        <f aca="false">B20/(1-$H$2)*F20/G20</f>
+        <v>-53.4245404359705</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>-130</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="E21" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <f aca="false">E21/(1-(1/(1+E21)^C21))</f>
+        <v>0.106079248252634</v>
+      </c>
+      <c r="G21" s="3" t="n">
+        <f aca="false">F21/(1-(1/(1+F21)^D21))</f>
+        <v>0.151161597709284</v>
+      </c>
+      <c r="I21" s="4" t="n">
+        <f aca="false">B21/(1-$H$2)*F21/G21</f>
+        <v>-122.850624134882</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>-90</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <f aca="false">E22/(1-(1/(1+E22)^C22))</f>
+        <v>0.106079248252634</v>
+      </c>
+      <c r="G22" s="3" t="n">
+        <f aca="false">F22/(1-(1/(1+F22)^D22))</f>
+        <v>0.167019608595705</v>
+      </c>
+      <c r="I22" s="4" t="n">
+        <f aca="false">B22/(1-$H$2)*F22/G22</f>
+        <v>-76.9751486618614</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>-90</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E23" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F23" s="3" t="n">
+        <f aca="false">E23/(1-(1/(1+E23)^C23))</f>
+        <v>0.106079248252634</v>
+      </c>
+      <c r="G23" s="3" t="n">
+        <f aca="false">F23/(1-(1/(1+F23)^D23))</f>
+        <v>0.167019608595705</v>
+      </c>
+      <c r="I23" s="4" t="n">
+        <f aca="false">B23/(1-$H$2)*F23/G23</f>
+        <v>-76.9751486618614</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>-90</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E24" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F24" s="3" t="n">
+        <f aca="false">E24/(1-(1/(1+E24)^C24))</f>
+        <v>0.106079248252634</v>
+      </c>
+      <c r="G24" s="3" t="n">
+        <f aca="false">F24/(1-(1/(1+F24)^D24))</f>
+        <v>0.167019608595705</v>
+      </c>
+      <c r="I24" s="4" t="n">
+        <f aca="false">B24/(1-$H$2)*F24/G24</f>
         <v>-76.9751486618614</v>
       </c>
     </row>
@@ -890,8 +1112,8 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="1" sqref="I10:J21 H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -901,7 +1123,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -922,12 +1144,12 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>-30</v>

</xml_diff>

<commit_message>
Proper accounting of tax credits for CC retrofits after introduction of parallel routes for CO2 storage (#119)
* Proper accounting of tax credits for CC retrofits after introduction of parallel routes for CO2 storage

* Update release notes

* apply usage-only 45Q credits for CC and DAC, unify credit logic across regimes and update eligible CO2 bus detection

* Add filter for regime and review co2 bus used to determine eligibility

* Select correct regime (IRA 2022 or OB3) if present

* Include empty regime cells in tax credits application

* Correct credits values IRA 2022
</commit_message>
<xml_diff>
--- a/data/tax_credits/tax_credits_calculations.xlsx
+++ b/data/tax_credits/tax_credits_calculations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="production_tax_credits" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t xml:space="preserve">carrier</t>
   </si>
@@ -50,6 +50,9 @@
     <t xml:space="preserve">levelized tax credit ($/output unit)</t>
   </si>
   <si>
+    <t xml:space="preserve">regime</t>
+  </si>
+  <si>
     <t xml:space="preserve">nuclear_existing</t>
   </si>
   <si>
@@ -77,6 +80,9 @@
     <t xml:space="preserve">ethanol from starch CC</t>
   </si>
   <si>
+    <t xml:space="preserve">OB3</t>
+  </si>
+  <si>
     <t xml:space="preserve">SMR CC</t>
   </si>
   <si>
@@ -90,6 +96,9 @@
   </si>
   <si>
     <t xml:space="preserve">DAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRA 2022</t>
   </si>
   <si>
     <t xml:space="preserve">Alkaline electrolyzer large</t>
@@ -193,7 +202,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -328,10 +337,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J21" activeCellId="0" sqref="I10:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -375,10 +384,13 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>-15</v>
@@ -389,7 +401,7 @@
       <c r="D2" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="3" t="n">
         <v>0.0320752195121951</v>
       </c>
       <c r="F2" s="3" t="n">
@@ -410,7 +422,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>-27.5</v>
@@ -421,7 +433,7 @@
       <c r="D3" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="3" t="n">
         <v>0.0564730561021376</v>
       </c>
       <c r="F3" s="3" t="n">
@@ -439,7 +451,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>-27.5</v>
@@ -450,7 +462,7 @@
       <c r="D4" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="3" t="n">
         <v>0.051519516365778</v>
       </c>
       <c r="F4" s="3" t="n">
@@ -468,7 +480,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>-27.5</v>
@@ -479,7 +491,7 @@
       <c r="D5" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="3" t="n">
         <v>0.0538314857296738</v>
       </c>
       <c r="F5" s="3" t="n">
@@ -497,7 +509,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>-27.5</v>
@@ -508,7 +520,7 @@
       <c r="D6" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="3" t="n">
         <v>0.0438437157985803</v>
       </c>
       <c r="F6" s="3" t="n">
@@ -526,7 +538,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>-27.5</v>
@@ -537,7 +549,7 @@
       <c r="D7" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="3" t="n">
         <v>0.0519007613262936</v>
       </c>
       <c r="F7" s="3" t="n">
@@ -555,7 +567,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>-27.5</v>
@@ -566,7 +578,7 @@
       <c r="D8" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="3" t="n">
         <v>0.0515227657596506</v>
       </c>
       <c r="F8" s="3" t="n">
@@ -584,7 +596,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>-27.5</v>
@@ -595,7 +607,7 @@
       <c r="D9" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E9" s="2" t="n">
+      <c r="E9" s="3" t="n">
         <v>0.0515227657596506</v>
       </c>
       <c r="F9" s="3" t="n">
@@ -613,7 +625,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>-85</v>
@@ -639,10 +651,13 @@
         <f aca="false">B10/(1-$H$2)*F10/G10</f>
         <v>-75.6847656176249</v>
       </c>
+      <c r="J10" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>-85</v>
@@ -668,10 +683,13 @@
         <f aca="false">B11/(1-$H$2)*F11/G11</f>
         <v>-75.6847656176249</v>
       </c>
+      <c r="J11" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>-85</v>
@@ -697,10 +715,13 @@
         <f aca="false">B12/(1-$H$2)*F12/G12</f>
         <v>-75.6847656176249</v>
       </c>
+      <c r="J12" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>-85</v>
@@ -726,10 +747,13 @@
         <f aca="false">B13/(1-$H$2)*F13/G13</f>
         <v>-75.6847656176249</v>
       </c>
+      <c r="J13" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>-85</v>
@@ -755,10 +779,13 @@
         <f aca="false">B14/(1-$H$2)*F14/G14</f>
         <v>-75.6847656176249</v>
       </c>
+      <c r="J14" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>-180</v>
@@ -784,91 +811,286 @@
         <f aca="false">B15/(1-$H$2)*F15/G15</f>
         <v>-170.10086418676</v>
       </c>
+      <c r="J15" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>-90</v>
+        <v>-60</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>0.1</v>
+        <v>0.07</v>
       </c>
       <c r="F16" s="3" t="n">
         <f aca="false">E16/(1-(1/(1+E16)^C16))</f>
-        <v>0.106079248252634</v>
+        <v>0.0943929257432557</v>
       </c>
       <c r="G16" s="3" t="n">
         <f aca="false">F16/(1-(1/(1+F16)^D16))</f>
-        <v>0.167019608595705</v>
+        <v>0.142756193054826</v>
       </c>
       <c r="I16" s="4" t="n">
         <f aca="false">B16/(1-$H$2)*F16/G16</f>
-        <v>-76.9751486618614</v>
+        <v>-53.4245404359705</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>-90</v>
+        <v>-60</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>0.1</v>
+        <v>0.07</v>
       </c>
       <c r="F17" s="3" t="n">
         <f aca="false">E17/(1-(1/(1+E17)^C17))</f>
-        <v>0.106079248252634</v>
+        <v>0.0943929257432557</v>
       </c>
       <c r="G17" s="3" t="n">
         <f aca="false">F17/(1-(1/(1+F17)^D17))</f>
-        <v>0.167019608595705</v>
+        <v>0.142756193054826</v>
       </c>
       <c r="I17" s="4" t="n">
         <f aca="false">B17/(1-$H$2)*F17/G17</f>
-        <v>-76.9751486618614</v>
+        <v>-53.4245404359705</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>-90</v>
+        <v>-60</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>0.1</v>
+        <v>0.07</v>
       </c>
       <c r="F18" s="3" t="n">
         <f aca="false">E18/(1-(1/(1+E18)^C18))</f>
-        <v>0.106079248252634</v>
+        <v>0.0943929257432557</v>
       </c>
       <c r="G18" s="3" t="n">
         <f aca="false">F18/(1-(1/(1+F18)^D18))</f>
-        <v>0.167019608595705</v>
+        <v>0.142756193054826</v>
       </c>
       <c r="I18" s="4" t="n">
         <f aca="false">B18/(1-$H$2)*F18/G18</f>
+        <v>-53.4245404359705</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <f aca="false">E19/(1-(1/(1+E19)^C19))</f>
+        <v>0.0943929257432557</v>
+      </c>
+      <c r="G19" s="3" t="n">
+        <f aca="false">F19/(1-(1/(1+F19)^D19))</f>
+        <v>0.142756193054826</v>
+      </c>
+      <c r="I19" s="4" t="n">
+        <f aca="false">B19/(1-$H$2)*F19/G19</f>
+        <v>-53.4245404359705</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="E20" s="3" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="F20" s="3" t="n">
+        <f aca="false">E20/(1-(1/(1+E20)^C20))</f>
+        <v>0.0943929257432557</v>
+      </c>
+      <c r="G20" s="3" t="n">
+        <f aca="false">F20/(1-(1/(1+F20)^D20))</f>
+        <v>0.142756193054826</v>
+      </c>
+      <c r="I20" s="4" t="n">
+        <f aca="false">B20/(1-$H$2)*F20/G20</f>
+        <v>-53.4245404359705</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>-130</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="E21" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <f aca="false">E21/(1-(1/(1+E21)^C21))</f>
+        <v>0.106079248252634</v>
+      </c>
+      <c r="G21" s="3" t="n">
+        <f aca="false">F21/(1-(1/(1+F21)^D21))</f>
+        <v>0.151161597709284</v>
+      </c>
+      <c r="I21" s="4" t="n">
+        <f aca="false">B21/(1-$H$2)*F21/G21</f>
+        <v>-122.850624134882</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>-90</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <f aca="false">E22/(1-(1/(1+E22)^C22))</f>
+        <v>0.106079248252634</v>
+      </c>
+      <c r="G22" s="3" t="n">
+        <f aca="false">F22/(1-(1/(1+F22)^D22))</f>
+        <v>0.167019608595705</v>
+      </c>
+      <c r="I22" s="4" t="n">
+        <f aca="false">B22/(1-$H$2)*F22/G22</f>
+        <v>-76.9751486618614</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>-90</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E23" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F23" s="3" t="n">
+        <f aca="false">E23/(1-(1/(1+E23)^C23))</f>
+        <v>0.106079248252634</v>
+      </c>
+      <c r="G23" s="3" t="n">
+        <f aca="false">F23/(1-(1/(1+F23)^D23))</f>
+        <v>0.167019608595705</v>
+      </c>
+      <c r="I23" s="4" t="n">
+        <f aca="false">B23/(1-$H$2)*F23/G23</f>
+        <v>-76.9751486618614</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>-90</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E24" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F24" s="3" t="n">
+        <f aca="false">E24/(1-(1/(1+E24)^C24))</f>
+        <v>0.106079248252634</v>
+      </c>
+      <c r="G24" s="3" t="n">
+        <f aca="false">F24/(1-(1/(1+F24)^D24))</f>
+        <v>0.167019608595705</v>
+      </c>
+      <c r="I24" s="4" t="n">
+        <f aca="false">B24/(1-$H$2)*F24/G24</f>
         <v>-76.9751486618614</v>
       </c>
     </row>
@@ -890,8 +1112,8 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="1" sqref="I10:J21 H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -901,7 +1123,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -922,12 +1144,12 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>-30</v>

</xml_diff>